<commit_message>
Before making nomenclature changes to sim code.
</commit_message>
<xml_diff>
--- a/Data/YsData.xlsx
+++ b/Data/YsData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37ddb746d34bbf38/Documents/NC State/ST 695/R Models/Comparisons/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37ddb746d34bbf38/Documents/NC State/ST 695/R Models/SeqSplitPlot/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{1871E4C4-349C-C34A-B768-E58EF8499C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C50CD2C-AA44-4DE3-A124-8A7AAE1DC84D}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{1871E4C4-349C-C34A-B768-E58EF8499C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C85EABD6-8B00-4B68-9598-91D161C63CC1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,7 +184,7 @@
     <t>MW%</t>
   </si>
   <si>
-    <t>Draw Ratio Category</t>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -583,15 +583,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="140" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="15.08984375" customWidth="1"/>
-    <col min="4" max="4" width="24.453125" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" customWidth="1"/>
+    <col min="7" max="9" width="2.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" customWidth="1"/>
+    <col min="11" max="11" width="2.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6328125" customWidth="1"/>
+    <col min="13" max="13" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.35">
@@ -613,20 +631,20 @@
       <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>41</v>
@@ -691,10 +709,10 @@
         <v>-1</v>
       </c>
       <c r="H2" s="3">
-        <v>-1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I2" s="3">
-        <v>-0.99999999999999978</v>
+        <v>-1</v>
       </c>
       <c r="J2" s="3">
         <v>-1</v>
@@ -762,19 +780,19 @@
         <v>1.05</v>
       </c>
       <c r="G3" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H3" s="3">
-        <v>-1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I3" s="3">
-        <v>-0.99999999999999978</v>
+        <v>-1</v>
       </c>
       <c r="J3" s="3">
         <v>-1</v>
       </c>
       <c r="K3" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L3" s="3">
         <v>1</v>
@@ -839,16 +857,16 @@
         <v>-1</v>
       </c>
       <c r="H4" s="3">
-        <v>-1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I4" s="3">
-        <v>-0.99999999999999978</v>
+        <v>-1</v>
       </c>
       <c r="J4" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K4" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L4" s="3">
         <v>1</v>
@@ -910,16 +928,16 @@
         <v>3</v>
       </c>
       <c r="G5" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H5" s="3">
-        <v>-1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I5" s="3">
-        <v>-0.99999999999999978</v>
+        <v>-1</v>
       </c>
       <c r="J5" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K5" s="3">
         <v>1</v>
@@ -987,13 +1005,13 @@
         <v>-1</v>
       </c>
       <c r="H6" s="3">
-        <v>-1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I6" s="3">
-        <v>-0.99999999999999978</v>
+        <v>1</v>
       </c>
       <c r="J6" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K6" s="3">
         <v>-1</v>
@@ -1058,19 +1076,19 @@
         <v>2</v>
       </c>
       <c r="G7" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H7" s="3">
-        <v>-1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I7" s="3">
-        <v>-0.99999999999999978</v>
+        <v>1</v>
       </c>
       <c r="J7" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K7" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L7" s="3">
         <v>2</v>
@@ -1135,16 +1153,16 @@
         <v>-1</v>
       </c>
       <c r="H8" s="3">
-        <v>-1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I8" s="3">
-        <v>-0.99999999999999978</v>
+        <v>1</v>
       </c>
       <c r="J8" s="3">
         <v>1</v>
       </c>
       <c r="K8" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L8" s="3">
         <v>2</v>
@@ -1206,13 +1224,13 @@
         <v>2.1</v>
       </c>
       <c r="G9" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H9" s="3">
-        <v>-1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I9" s="3">
-        <v>-0.99999999999999978</v>
+        <v>1</v>
       </c>
       <c r="J9" s="3">
         <v>1</v>
@@ -1283,10 +1301,10 @@
         <v>-1</v>
       </c>
       <c r="H10" s="3">
-        <v>-1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I10" s="3">
-        <v>1.0000000000000002</v>
+        <v>-1</v>
       </c>
       <c r="J10" s="3">
         <v>-1</v>
@@ -1354,19 +1372,19 @@
         <v>2.5</v>
       </c>
       <c r="G11" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H11" s="3">
-        <v>-1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I11" s="3">
-        <v>1.0000000000000002</v>
+        <v>-1</v>
       </c>
       <c r="J11" s="3">
         <v>-1</v>
       </c>
       <c r="K11" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L11" s="3">
         <v>3</v>
@@ -1431,16 +1449,16 @@
         <v>-1</v>
       </c>
       <c r="H12" s="3">
-        <v>-1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I12" s="3">
-        <v>1.0000000000000002</v>
+        <v>-1</v>
       </c>
       <c r="J12" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K12" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L12" s="3">
         <v>3</v>
@@ -1502,16 +1520,16 @@
         <v>3.7</v>
       </c>
       <c r="G13" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H13" s="3">
-        <v>-1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I13" s="3">
-        <v>1.0000000000000002</v>
+        <v>-1</v>
       </c>
       <c r="J13" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K13" s="3">
         <v>1</v>
@@ -1579,13 +1597,13 @@
         <v>-1</v>
       </c>
       <c r="H14" s="3">
-        <v>-1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I14" s="3">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="J14" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K14" s="3">
         <v>-1</v>
@@ -1650,19 +1668,19 @@
         <v>3.88</v>
       </c>
       <c r="G15" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H15" s="3">
-        <v>-1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I15" s="3">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="J15" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K15" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L15" s="3">
         <v>4</v>
@@ -1727,16 +1745,16 @@
         <v>-1</v>
       </c>
       <c r="H16" s="3">
-        <v>-1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I16" s="3">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="J16" s="3">
         <v>1</v>
       </c>
       <c r="K16" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L16" s="3">
         <v>4</v>
@@ -1798,13 +1816,13 @@
         <v>2.8</v>
       </c>
       <c r="G17" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H17" s="3">
-        <v>-1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I17" s="3">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="J17" s="3">
         <v>1</v>
@@ -1871,19 +1889,19 @@
       <c r="F18" s="3">
         <v>1</v>
       </c>
-      <c r="G18" s="5">
-        <v>-1</v>
+      <c r="G18" s="3">
+        <v>1</v>
       </c>
       <c r="H18" s="3">
-        <v>1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I18" s="3">
-        <v>-0.99999999999999978</v>
+        <v>-1</v>
       </c>
       <c r="J18" s="3">
         <v>-1</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18" s="5">
         <v>-1</v>
       </c>
       <c r="L18" s="3">
@@ -1945,20 +1963,20 @@
       <c r="F19" s="3">
         <v>1.9</v>
       </c>
-      <c r="G19" s="6">
-        <v>-1</v>
+      <c r="G19" s="3">
+        <v>1</v>
       </c>
       <c r="H19" s="3">
-        <v>1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I19" s="3">
-        <v>-0.99999999999999978</v>
+        <v>-1</v>
       </c>
       <c r="J19" s="3">
-        <v>-1</v>
-      </c>
-      <c r="K19" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="K19" s="6">
+        <v>-1</v>
       </c>
       <c r="L19" s="3">
         <v>5</v>
@@ -2023,13 +2041,13 @@
         <v>1</v>
       </c>
       <c r="H20" s="3">
-        <v>1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I20" s="3">
-        <v>-0.99999999999999978</v>
+        <v>-1</v>
       </c>
       <c r="J20" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K20" s="3">
         <v>1</v>
@@ -2094,16 +2112,16 @@
         <v>1.05</v>
       </c>
       <c r="G21" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H21" s="3">
-        <v>1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I21" s="3">
-        <v>-0.99999999999999978</v>
+        <v>1</v>
       </c>
       <c r="J21" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K21" s="3">
         <v>-1</v>
@@ -2171,16 +2189,16 @@
         <v>1</v>
       </c>
       <c r="H22" s="3">
-        <v>1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I22" s="3">
-        <v>-0.99999999999999978</v>
+        <v>1</v>
       </c>
       <c r="J22" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K22" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L22" s="3">
         <v>6</v>
@@ -2242,19 +2260,19 @@
         <v>1.3</v>
       </c>
       <c r="G23" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H23" s="3">
-        <v>1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I23" s="3">
-        <v>-0.99999999999999978</v>
+        <v>1</v>
       </c>
       <c r="J23" s="3">
         <v>1</v>
       </c>
       <c r="K23" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L23" s="3">
         <v>6</v>
@@ -2319,10 +2337,10 @@
         <v>1</v>
       </c>
       <c r="H24" s="3">
-        <v>1</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="I24" s="3">
-        <v>-0.99999999999999978</v>
+        <v>1</v>
       </c>
       <c r="J24" s="3">
         <v>1</v>
@@ -2390,13 +2408,13 @@
         <v>1</v>
       </c>
       <c r="G25" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H25" s="3">
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I25" s="3">
-        <v>1.0000000000000002</v>
+        <v>-1</v>
       </c>
       <c r="J25" s="3">
         <v>-1</v>
@@ -2467,16 +2485,16 @@
         <v>1</v>
       </c>
       <c r="H26" s="3">
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I26" s="3">
-        <v>1.0000000000000002</v>
+        <v>-1</v>
       </c>
       <c r="J26" s="3">
         <v>-1</v>
       </c>
       <c r="K26" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L26" s="3">
         <v>7</v>
@@ -2538,19 +2556,19 @@
         <v>2.7</v>
       </c>
       <c r="G27" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H27" s="3">
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I27" s="3">
-        <v>1.0000000000000002</v>
+        <v>-1</v>
       </c>
       <c r="J27" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K27" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L27" s="3">
         <v>7</v>
@@ -2615,13 +2633,13 @@
         <v>1</v>
       </c>
       <c r="H28" s="3">
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I28" s="3">
-        <v>1.0000000000000002</v>
+        <v>-1</v>
       </c>
       <c r="J28" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K28" s="3">
         <v>1</v>
@@ -2686,16 +2704,16 @@
         <v>1</v>
       </c>
       <c r="G29" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H29" s="3">
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I29" s="3">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="J29" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K29" s="3">
         <v>-1</v>
@@ -2763,16 +2781,16 @@
         <v>1</v>
       </c>
       <c r="H30" s="3">
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I30" s="3">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="J30" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K30" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L30" s="3">
         <v>8</v>
@@ -2834,19 +2852,19 @@
         <v>2.13</v>
       </c>
       <c r="G31" s="3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H31" s="3">
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I31" s="3">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="J31" s="3">
         <v>1</v>
       </c>
       <c r="K31" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L31" s="3">
         <v>8</v>
@@ -2911,10 +2929,10 @@
         <v>1</v>
       </c>
       <c r="H32" s="3">
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I32" s="3">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="J32" s="3">
         <v>1</v>
@@ -2964,12 +2982,13 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X32">
+    <sortCondition ref="G2:G32"/>
     <sortCondition ref="H2:H32"/>
     <sortCondition ref="I2:I32"/>
     <sortCondition ref="J2:J32"/>
-    <sortCondition ref="K2:K32"/>
     <sortCondition ref="F2:F32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>